<commit_message>
Mock Test Student List updated
Mock Test Student List updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/CollegeDoors/MockTest/MockTest-Students.xlsx
+++ b/Offline/BusinessManagement/Information/CollegeDoors/MockTest/MockTest-Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\CollegeDoors\MockTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3160AEF6-B8B6-4BE2-9BD7-BA2ED837CCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ED87B7-301F-4E5A-B2E5-7FEB08387306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>tc={DF1E2BD4-72C6-4700-BFFC-3C8B6EB0033C}</author>
   </authors>
   <commentList>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{DF1E2BD4-72C6-4700-BFFC-3C8B6EB0033C}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{DF1E2BD4-72C6-4700-BFFC-3C8B6EB0033C}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>SlNo</t>
   </si>
@@ -83,13 +83,25 @@
   </si>
   <si>
     <t>ICSE</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Std X</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Rahul Dutta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,12 +116,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,7 +456,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G3" dT="2023-11-14T06:10:03.53" personId="{A19D380A-A92E-4E11-9670-DD97CAE0762B}" id="{DF1E2BD4-72C6-4700-BFFC-3C8B6EB0033C}">
+  <threadedComment ref="H3" dT="2023-11-14T06:10:03.53" personId="{A19D380A-A92E-4E11-9670-DD97CAE0762B}" id="{DF1E2BD4-72C6-4700-BFFC-3C8B6EB0033C}">
     <text xml:space="preserve">1) English
 2) French
 3) Physics
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,10 +484,12 @@
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -501,13 +509,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -523,8 +537,14 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="2">
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
         <v>45256</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>